<commit_message>
Change from others to zeroing problem
</commit_message>
<xml_diff>
--- a/data/misused_bar_graph_figures/sci_signal/zero/annotation.xlsx
+++ b/data/misused_bar_graph_figures/sci_signal/zero/annotation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tlin/Files/2023-2028-UC_Berkeley/_landry-lab/research-project/local/misused-bar-graphs/data/misused_bar_graph_figures/sci_signal/zero/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD1E2BB9-476D-674D-9662-815EEA6B6917}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B847F818-1373-2B47-BAA2-EAC31A969C34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="800" yWindow="500" windowWidth="18800" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19600" yWindow="500" windowWidth="18800" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="111">
   <si>
     <t>DOI</t>
   </si>
@@ -338,6 +338,21 @@
   </si>
   <si>
     <t>Concentration</t>
+  </si>
+  <si>
+    <t>10.1126:scisignal.add0509_zero_fig3</t>
+  </si>
+  <si>
+    <t>10.1126:scisignal.abq3362_zero_fig1</t>
+  </si>
+  <si>
+    <t>10.1126:scisignal.abq3362</t>
+  </si>
+  <si>
+    <t>Percents of CD206+ cells</t>
+  </si>
+  <si>
+    <t>Cell percentage</t>
   </si>
 </sst>
 </file>
@@ -738,10 +753,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="211" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD17"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="211" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1173,10 +1188,10 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>83</v>
+        <v>107</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>108</v>
       </c>
       <c r="C13" t="s">
         <v>5</v>
@@ -1188,19 +1203,19 @@
         <v>7</v>
       </c>
       <c r="F13" t="s">
-        <v>37</v>
+        <v>109</v>
       </c>
       <c r="G13" t="s">
         <v>60</v>
       </c>
       <c r="H13" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I13" t="s">
-        <v>63</v>
+        <v>110</v>
       </c>
       <c r="J13" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="K13" t="s">
         <v>59</v>
@@ -1208,7 +1223,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B14" t="s">
         <v>16</v>
@@ -1217,7 +1232,7 @@
         <v>5</v>
       </c>
       <c r="D14" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E14" t="s">
         <v>7</v>
@@ -1243,34 +1258,34 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E15" t="s">
         <v>7</v>
       </c>
       <c r="F15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G15" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="H15" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="I15" t="s">
-        <v>103</v>
+        <v>63</v>
       </c>
       <c r="J15" t="s">
-        <v>103</v>
+        <v>63</v>
       </c>
       <c r="K15" t="s">
         <v>59</v>
@@ -1278,7 +1293,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B16" t="s">
         <v>17</v>
@@ -1287,13 +1302,13 @@
         <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E16" t="s">
         <v>7</v>
       </c>
       <c r="F16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G16" t="s">
         <v>56</v>
@@ -1302,7 +1317,7 @@
         <v>57</v>
       </c>
       <c r="I16" t="s">
-        <v>58</v>
+        <v>103</v>
       </c>
       <c r="J16" t="s">
         <v>103</v>
@@ -1313,34 +1328,34 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C17" t="s">
         <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E17" t="s">
         <v>7</v>
       </c>
       <c r="F17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G17" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H17" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="I17" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="J17" t="s">
-        <v>63</v>
+        <v>103</v>
       </c>
       <c r="K17" t="s">
         <v>59</v>
@@ -1348,34 +1363,34 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>88</v>
+        <v>106</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C18" t="s">
         <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E18" t="s">
         <v>7</v>
       </c>
       <c r="F18" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G18" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H18" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="I18" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="J18" t="s">
-        <v>63</v>
+        <v>103</v>
       </c>
       <c r="K18" t="s">
         <v>59</v>
@@ -1383,10 +1398,10 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C19" t="s">
         <v>5</v>
@@ -1398,19 +1413,19 @@
         <v>7</v>
       </c>
       <c r="F19" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G19" t="s">
         <v>60</v>
       </c>
       <c r="H19" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="I19" t="s">
-        <v>103</v>
+        <v>63</v>
       </c>
       <c r="J19" t="s">
-        <v>103</v>
+        <v>63</v>
       </c>
       <c r="K19" t="s">
         <v>59</v>
@@ -1418,34 +1433,34 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C20" t="s">
         <v>5</v>
       </c>
       <c r="D20" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E20" t="s">
         <v>7</v>
       </c>
       <c r="F20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G20" t="s">
         <v>60</v>
       </c>
       <c r="H20" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="I20" t="s">
-        <v>103</v>
+        <v>63</v>
       </c>
       <c r="J20" t="s">
-        <v>103</v>
+        <v>63</v>
       </c>
       <c r="K20" t="s">
         <v>59</v>
@@ -1453,10 +1468,10 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C21" t="s">
         <v>5</v>
@@ -1468,19 +1483,19 @@
         <v>7</v>
       </c>
       <c r="F21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G21" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="H21" t="s">
         <v>57</v>
       </c>
       <c r="I21" t="s">
-        <v>66</v>
+        <v>103</v>
       </c>
       <c r="J21" t="s">
-        <v>66</v>
+        <v>103</v>
       </c>
       <c r="K21" t="s">
         <v>59</v>
@@ -1488,10 +1503,10 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C22" t="s">
         <v>5</v>
@@ -1503,19 +1518,19 @@
         <v>7</v>
       </c>
       <c r="F22" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G22" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="H22" t="s">
         <v>57</v>
       </c>
       <c r="I22" t="s">
-        <v>66</v>
+        <v>103</v>
       </c>
       <c r="J22" t="s">
-        <v>66</v>
+        <v>103</v>
       </c>
       <c r="K22" t="s">
         <v>59</v>
@@ -1523,10 +1538,10 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C23" t="s">
         <v>5</v>
@@ -1538,19 +1553,19 @@
         <v>7</v>
       </c>
       <c r="F23" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G23" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H23" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="I23" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="J23" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="K23" t="s">
         <v>59</v>
@@ -1558,10 +1573,10 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C24" t="s">
         <v>5</v>
@@ -1573,19 +1588,19 @@
         <v>7</v>
       </c>
       <c r="F24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G24" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H24" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="I24" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="J24" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="K24" t="s">
         <v>59</v>
@@ -1593,7 +1608,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B25" t="s">
         <v>22</v>
@@ -1602,13 +1617,13 @@
         <v>5</v>
       </c>
       <c r="D25" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E25" t="s">
         <v>7</v>
       </c>
       <c r="F25" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G25" t="s">
         <v>60</v>
@@ -1628,34 +1643,34 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C26" t="s">
         <v>5</v>
       </c>
       <c r="D26" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E26" t="s">
         <v>7</v>
       </c>
       <c r="F26" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G26" t="s">
         <v>60</v>
       </c>
       <c r="H26" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="I26" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="J26" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="K26" t="s">
         <v>59</v>
@@ -1663,34 +1678,34 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C27" t="s">
         <v>5</v>
       </c>
       <c r="D27" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E27" t="s">
         <v>7</v>
       </c>
       <c r="F27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G27" t="s">
         <v>60</v>
       </c>
       <c r="H27" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="I27" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="J27" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="K27" t="s">
         <v>59</v>
@@ -1698,7 +1713,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B28" t="s">
         <v>23</v>
@@ -1707,7 +1722,7 @@
         <v>5</v>
       </c>
       <c r="D28" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E28" t="s">
         <v>7</v>
@@ -1733,7 +1748,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B29" t="s">
         <v>23</v>
@@ -1742,7 +1757,7 @@
         <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E29" t="s">
         <v>7</v>
@@ -1768,69 +1783,69 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B30" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C30" t="s">
         <v>5</v>
       </c>
       <c r="D30" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E30" t="s">
         <v>7</v>
       </c>
       <c r="F30" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G30" t="s">
         <v>60</v>
       </c>
       <c r="H30" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="I30" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="J30" t="s">
-        <v>63</v>
-      </c>
-      <c r="K30">
-        <v>10</v>
+        <v>69</v>
+      </c>
+      <c r="K30" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B31" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C31" t="s">
         <v>5</v>
       </c>
       <c r="D31" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="E31" t="s">
         <v>7</v>
       </c>
       <c r="F31" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G31" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="H31" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="I31" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="J31" t="s">
-        <v>103</v>
+        <v>69</v>
       </c>
       <c r="K31" t="s">
         <v>59</v>
@@ -1838,36 +1853,106 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B32" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32" t="s">
+        <v>49</v>
+      </c>
+      <c r="G32" t="s">
+        <v>60</v>
+      </c>
+      <c r="H32" t="s">
+        <v>63</v>
+      </c>
+      <c r="I32" t="s">
+        <v>63</v>
+      </c>
+      <c r="J32" t="s">
+        <v>63</v>
+      </c>
+      <c r="K32">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B33" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" t="s">
+        <v>7</v>
+      </c>
+      <c r="F33" t="s">
+        <v>50</v>
+      </c>
+      <c r="G33" t="s">
+        <v>56</v>
+      </c>
+      <c r="H33" t="s">
+        <v>57</v>
+      </c>
+      <c r="I33" t="s">
+        <v>62</v>
+      </c>
+      <c r="J33" t="s">
+        <v>103</v>
+      </c>
+      <c r="K33" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B34" t="s">
         <v>25</v>
       </c>
-      <c r="C32" t="s">
-        <v>5</v>
-      </c>
-      <c r="D32" t="s">
+      <c r="C34" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" t="s">
         <v>9</v>
       </c>
-      <c r="E32" t="s">
-        <v>7</v>
-      </c>
-      <c r="F32" t="s">
+      <c r="E34" t="s">
+        <v>7</v>
+      </c>
+      <c r="F34" t="s">
         <v>50</v>
       </c>
-      <c r="G32" t="s">
+      <c r="G34" t="s">
         <v>56</v>
       </c>
-      <c r="H32" t="s">
+      <c r="H34" t="s">
         <v>57</v>
       </c>
-      <c r="I32" t="s">
+      <c r="I34" t="s">
         <v>62</v>
       </c>
-      <c r="J32" t="s">
+      <c r="J34" t="s">
         <v>103</v>
       </c>
-      <c r="K32" t="s">
+      <c r="K34" t="s">
         <v>59</v>
       </c>
     </row>

</xml_diff>